<commit_message>
added excel files and review files
</commit_message>
<xml_diff>
--- a/assets/misc/Example2_Solution.xlsx
+++ b/assets/misc/Example2_Solution.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Flowershop sales" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Flowershop sales'!$A$6:$K$17</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -307,7 +307,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -330,11 +330,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,14 +361,37 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -389,11 +421,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -484,6 +511,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -519,6 +563,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -697,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -727,35 +788,35 @@
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="7">
         <f ca="1">TODAY()</f>
-        <v>42104</v>
+        <v>42830</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1253,8 +1314,11 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E5:E14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1267,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1294,10 +1358,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B2">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C2" s="3" t="str">
         <f>VLOOKUP(B2,Grades!$A$4:$B$8,2,TRUE)</f>
@@ -1310,26 +1374,26 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C3" s="3" t="str">
         <f>VLOOKUP(B3,Grades!$A$4:$B$8,2,TRUE)</f>
-        <v>B</v>
+        <v>A</v>
       </c>
       <c r="D3" s="3" t="str">
         <f>VLOOKUP(C3,Grades!$A$13:$B$17,2,TRUE)</f>
-        <v>Credit</v>
+        <v>Distinction</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="str">
         <f>VLOOKUP(B4,Grades!$A$4:$B$8,2,TRUE)</f>
@@ -1342,42 +1406,42 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="str">
         <f>VLOOKUP(B5,Grades!$A$4:$B$8,2,TRUE)</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="D5" s="3" t="str">
         <f>VLOOKUP(C5,Grades!$A$13:$B$17,2,TRUE)</f>
-        <v>Pass</v>
+        <v>Distinction</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>VLOOKUP(B6,Grades!$A$4:$B$8,2,TRUE)</f>
-        <v>A</v>
+        <v>B</v>
       </c>
       <c r="D6" s="3" t="str">
         <f>VLOOKUP(C6,Grades!$A$13:$B$17,2,TRUE)</f>
-        <v>Distinction</v>
+        <v>Credit</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B7">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3" t="str">
         <f>VLOOKUP(B7,Grades!$A$4:$B$8,2,TRUE)</f>
@@ -1390,10 +1454,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B8">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="str">
         <f>VLOOKUP(B8,Grades!$A$4:$B$8,2,TRUE)</f>
@@ -1406,26 +1470,26 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3" t="str">
         <f>VLOOKUP(B9,Grades!$A$4:$B$8,2,TRUE)</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="D9" s="3" t="str">
         <f>VLOOKUP(C9,Grades!$A$13:$B$17,2,TRUE)</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B10">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3" t="str">
         <f>VLOOKUP(B10,Grades!$A$4:$B$8,2,TRUE)</f>
@@ -1438,18 +1502,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B11">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C11" s="3" t="str">
         <f>VLOOKUP(B11,Grades!$A$4:$B$8,2,TRUE)</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="D11" s="3" t="str">
         <f>VLOOKUP(C11,Grades!$A$13:$B$17,2,TRUE)</f>
-        <v>Distinction</v>
+        <v>Fail</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1472,7 +1536,7 @@
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="13">
         <f>AVERAGE(B2:B12)</f>
         <v>77.090909090909093</v>
       </c>
@@ -1559,16 +1623,19 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D12">
+    <sortCondition descending="1" ref="B2:B12"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2:B12">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>65</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>65</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1705,25 +1772,25 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="26" spans="1:8" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">

</xml_diff>